<commit_message>
peaufinage du portfolio pour l'E4
</commit_message>
<xml_diff>
--- a/documents/E4_Tableau_Competences.xlsx
+++ b/documents/E4_Tableau_Competences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quens\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projet NetBeans\Mon Portfolio SIO\MonPortfolioSIO\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A340F04D-BA18-44E8-BA99-3122CBA26E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1847B14A-E0B4-4EB3-B9CA-0FFCE4A49184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$2:$H$32</definedName>
   </definedNames>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -108,9 +108,6 @@
 (intitulé et liste des documents et productions associés)</t>
   </si>
   <si>
-    <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
@@ -129,12 +126,6 @@
     <t>Centre de formation : CNED Poitiers</t>
   </si>
   <si>
-    <t>AP3 2é année Mediatek86 : évolution d'une application de bureau en C# avec qualité de code, accès avec authentification, tests unitaires et fonctionnels, logs, mise en ligne de la BDD, création d'un installeur : gestion des documents de la médiathèque Mediatek86 (code source, BDD, tests unitaires et fonctionnels, fichier de logs, documentation technique, vidéo documentation utilisateur, compte rendu d'activité)</t>
-  </si>
-  <si>
-    <t>Réalisation du stage en Entrerpise de 1er année : Création et intégration d'un quiz des connaissances dans une page web, mise à jour de l'interface des pages du site web avec le nouveau contenu de la charte graphique, optimisation du SEO, création et incorporation des questionnaires de formations, création et intégration d'un teaser video de formations (compte rendu d'activité, site map du site, lien du site web, video teaser)</t>
-  </si>
-  <si>
     <t>Denombrement C# console : Récupération d'un programme, analyse des défaillances, énumération des dysfonctionnements et correction proposée, correction du code (Code source, code corrigé, tableau de dysfonctionnements)</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>Mise en place de la veille technologique, du profil professionnel et des besoins en formation(carte heuristique d'un métier, portfolio, veille technologique, profil LinkedIn)</t>
   </si>
   <si>
-    <t>Réalisation stage en entrerpise 2é année : création d'une application de bureau en C# avec qualité de code, accès avec authentification, mise en ligne de la BDD, création d'un installeur : Systeme de gestion des adhérents (S.A.G.A) Gestion adhérents : Permettre de s'authentifier, créer un nouvel adhérent, consulter son historique d'activité, recharger son solde de crédits, Gérer les consommables et les coût : accès au consommables exitantn faire des recherche de consommable, les modifier, pourvoir en créer, etc ... Prestation : Consulter, modifer ou créer des prestations ou des types de prestation avec leurs sous catégories (code source, BDD, documentation technique, compte rendu d'activité)</t>
-  </si>
-  <si>
     <t>15/09/2021 au 03/11/2021</t>
   </si>
   <si>
@@ -165,13 +153,7 @@
     <t>x</t>
   </si>
   <si>
-    <t xml:space="preserve">Création et intégration d'un quiz, et de plusieurs formulaires de test de connaissance </t>
-  </si>
-  <si>
     <t>Création d'une application de bureau C#</t>
-  </si>
-  <si>
-    <t>Création de diverses documentations (documentation technique, besoins de la BDD, Projet d'évolution, cas d'utilisation)</t>
   </si>
   <si>
     <t>Création et mise en ligne d'une base de données (avec MCD)</t>
@@ -202,6 +184,27 @@
   <si>
     <t>NOM et prénom : Stachowiak Quentin</t>
   </si>
+  <si>
+    <t>Mon portfolio : https://micro530.github.io</t>
+  </si>
+  <si>
+    <t>N° candidat : 02143489128</t>
+  </si>
+  <si>
+    <t>AP3 2éme année Mediatek86 : évolution d'une application de bureau en C# avec qualité de code, accès avec authentification, tests unitaires et fonctionnels, logs, mise en ligne de la BDD, création d'un installeur : gestion des documents de la médiathèque Mediatek86 (code source, BDD, tests unitaires et fonctionnels, fichier de logs, documentation technique, vidéo documentation utilisateur, compte rendu d'activité)</t>
+  </si>
+  <si>
+    <t>Réalisation stage en entrerpise 2éme année : création d'une application de bureau en C# avec qualité de code, accès avec authentification, mise en ligne de la BDD, création d'un installeur : Système de gestion des adhérents (S.A.G.A) Gestion adhérents : Permettre de s'authentifier, créer un nouvel adhérent, consulter son historique d'activité, recharger son solde de crédits, Gérer les consommables et les coûts : accès au consommables exitant, faire des recherches de consommable, les modifier, pourvoir en créer, etc ... Prestation : Consulter, modifier ou créer des prestations ou des types de prestation avec leurs sous-catégories (code source, BDD, documentation technique, compte rendu d'activité)</t>
+  </si>
+  <si>
+    <t>Réalisation du stage en Entreprise de 1er année : Création et intégration d'un quiz des connaissances dans une page web, mise à jour de l'interface des pages du site web avec le nouveau contenu de la charte graphique, optimisation du SEO, création et incorporation des questionnaires de formations, création et intégration d'un teaser vidéo de formations (compte-rendu d'activité, sitemap du site, lien du site web, vidéo teaser)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création et intégration d'un quiz, et de plusieurs formulaires de tests de connaissances </t>
+  </si>
+  <si>
+    <t>Création de diverses documentations (documentation technique, besoins de la BDD, Projet d'évolution, cas d'utilisations)</t>
+  </si>
 </sst>
 </file>
 
@@ -210,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -273,13 +276,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="19">
@@ -547,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -621,15 +638,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,14 +680,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,10 +1025,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ77"/>
+  <dimension ref="A1:AQ78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1020,161 +1040,126 @@
     <col min="44" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:43" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:43" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:43" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="27"/>
-    </row>
-    <row r="2" spans="1:43" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="1:43" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="36" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:43" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:43" s="2" customFormat="1" ht="325.14999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="8" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.14999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-      <c r="AH6"/>
-      <c r="AI6"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1211,25 +1196,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="20"/>
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1266,23 +1243,23 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9"/>
@@ -1321,20 +1298,24 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="19"/>
+        <v>29</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="H10" s="20"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1372,18 +1353,18 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="19"/>
-      <c r="D11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="20"/>
@@ -1423,21 +1404,21 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="H12" s="20"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1474,17 +1455,21 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1521,19 +1506,17 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1570,15 +1553,15 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -1619,12 +1602,16 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="B16" s="10"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="E16" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
@@ -1889,17 +1876,15 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -1936,23 +1921,17 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="20"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -1991,14 +1970,20 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B24" s="10"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="H24" s="20"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -2036,18 +2021,16 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="G25" s="19"/>
       <c r="H25" s="20"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -2085,9 +2068,9 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="19"/>
@@ -2095,7 +2078,7 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26"/>
@@ -2135,13 +2118,17 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
+      <c r="A27" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="B27" s="10"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="G27" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="H27" s="20"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -2180,14 +2167,14 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2269,15 +2256,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="22"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2314,15 +2301,15 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="24"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2359,7 +2346,51 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+      <c r="AC32"/>
+      <c r="AD32"/>
+      <c r="AE32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32"/>
+    </row>
     <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2405,24 +2436,26 @@
     <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:F2"/>
     <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>